<commit_message>
update code delete staff
</commit_message>
<xml_diff>
--- a/public/excels/excel_template.xlsx
+++ b/public/excels/excel_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF91AAD7-9BE7-B84C-A086-25D68A9391E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997FF0B3-7194-0F41-AFD5-DBB359B25369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15840" xr2:uid="{75868DF0-7A29-984B-89E5-7B62FCADAA08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A9604F44-8D92-214B-BC6B-474F2C1DADC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,28 +25,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Danh sách công việc</t>
+  </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>detail</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>status</t>
+    <t>Chi tết công việc
+(detail)</t>
+  </si>
+  <si>
+    <t>Ngày kết thúc
+(end_date)</t>
+  </si>
+  <si>
+    <t>Ngày bắt đầu
+(start_date)</t>
+  </si>
+  <si>
+    <t>Trạng thái
+(end_date)</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày (date): </t>
+  </si>
+  <si>
+    <t>Nhân viên ( staff) :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,16 +70,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="23"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -71,12 +120,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,33 +484,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D0BF8A-7F9A-784C-AB77-E80059BBD756}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8566A97E-606A-1D4C-B1ED-C7208C8C1BD1}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>